<commit_message>
Rename class_period to section and add multi-section Canvas support
- Rename `class_period` column to `section` across all sheets and code
- Add `getCanvasSections()` to fetch section data from Canvas API
- Include enrollment data in student fetch for auto-section assignment
- Teachers no longer need to manually specify sections — students are
  auto-assigned to their Canvas section during roster sync
- Update filename parser to support "Section N" format (legacy "Period N" still works)
- Regenerate template.xlsx with updated column names

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,11 +35,6 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <i val="1"/>
-      <color rgb="00888888"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -56,7 +51,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -64,26 +59,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <right style="thin">
-        <color rgb="00E0E0E0"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="00E0E0E0"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -459,7 +442,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="28" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -590,27 +573,6 @@
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Instructions: Edit setting_value cells above. mode = 'group' or 'individual'.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>distribute_email / distribute_canvas = 'true' or 'false'.</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>API keys go in Script Properties (File &gt; Project Properties), not here.</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -623,7 +585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -632,18 +594,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
     <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="40" customWidth="1" min="8" max="8"/>
-    <col width="40" customWidth="1" min="9" max="9"/>
-    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="22" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
     <col width="24" customWidth="1" min="11" max="11"/>
-    <col width="40" customWidth="1" min="12" max="12"/>
+    <col width="17" customWidth="1" min="12" max="12"/>
     <col width="14" customWidth="1" min="13" max="13"/>
     <col width="14" customWidth="1" min="14" max="14"/>
   </cols>
@@ -661,7 +623,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>class_period</t>
+          <t>section</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -720,9 +682,1009 @@
         </is>
       </c>
     </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+    <row r="247"/>
+    <row r="248"/>
+    <row r="249"/>
+    <row r="250"/>
+    <row r="251"/>
+    <row r="252"/>
+    <row r="253"/>
+    <row r="254"/>
+    <row r="255"/>
+    <row r="256"/>
+    <row r="257"/>
+    <row r="258"/>
+    <row r="259"/>
+    <row r="260"/>
+    <row r="261"/>
+    <row r="262"/>
+    <row r="263"/>
+    <row r="264"/>
+    <row r="265"/>
+    <row r="266"/>
+    <row r="267"/>
+    <row r="268"/>
+    <row r="269"/>
+    <row r="270"/>
+    <row r="271"/>
+    <row r="272"/>
+    <row r="273"/>
+    <row r="274"/>
+    <row r="275"/>
+    <row r="276"/>
+    <row r="277"/>
+    <row r="278"/>
+    <row r="279"/>
+    <row r="280"/>
+    <row r="281"/>
+    <row r="282"/>
+    <row r="283"/>
+    <row r="284"/>
+    <row r="285"/>
+    <row r="286"/>
+    <row r="287"/>
+    <row r="288"/>
+    <row r="289"/>
+    <row r="290"/>
+    <row r="291"/>
+    <row r="292"/>
+    <row r="293"/>
+    <row r="294"/>
+    <row r="295"/>
+    <row r="296"/>
+    <row r="297"/>
+    <row r="298"/>
+    <row r="299"/>
+    <row r="300"/>
+    <row r="301"/>
+    <row r="302"/>
+    <row r="303"/>
+    <row r="304"/>
+    <row r="305"/>
+    <row r="306"/>
+    <row r="307"/>
+    <row r="308"/>
+    <row r="309"/>
+    <row r="310"/>
+    <row r="311"/>
+    <row r="312"/>
+    <row r="313"/>
+    <row r="314"/>
+    <row r="315"/>
+    <row r="316"/>
+    <row r="317"/>
+    <row r="318"/>
+    <row r="319"/>
+    <row r="320"/>
+    <row r="321"/>
+    <row r="322"/>
+    <row r="323"/>
+    <row r="324"/>
+    <row r="325"/>
+    <row r="326"/>
+    <row r="327"/>
+    <row r="328"/>
+    <row r="329"/>
+    <row r="330"/>
+    <row r="331"/>
+    <row r="332"/>
+    <row r="333"/>
+    <row r="334"/>
+    <row r="335"/>
+    <row r="336"/>
+    <row r="337"/>
+    <row r="338"/>
+    <row r="339"/>
+    <row r="340"/>
+    <row r="341"/>
+    <row r="342"/>
+    <row r="343"/>
+    <row r="344"/>
+    <row r="345"/>
+    <row r="346"/>
+    <row r="347"/>
+    <row r="348"/>
+    <row r="349"/>
+    <row r="350"/>
+    <row r="351"/>
+    <row r="352"/>
+    <row r="353"/>
+    <row r="354"/>
+    <row r="355"/>
+    <row r="356"/>
+    <row r="357"/>
+    <row r="358"/>
+    <row r="359"/>
+    <row r="360"/>
+    <row r="361"/>
+    <row r="362"/>
+    <row r="363"/>
+    <row r="364"/>
+    <row r="365"/>
+    <row r="366"/>
+    <row r="367"/>
+    <row r="368"/>
+    <row r="369"/>
+    <row r="370"/>
+    <row r="371"/>
+    <row r="372"/>
+    <row r="373"/>
+    <row r="374"/>
+    <row r="375"/>
+    <row r="376"/>
+    <row r="377"/>
+    <row r="378"/>
+    <row r="379"/>
+    <row r="380"/>
+    <row r="381"/>
+    <row r="382"/>
+    <row r="383"/>
+    <row r="384"/>
+    <row r="385"/>
+    <row r="386"/>
+    <row r="387"/>
+    <row r="388"/>
+    <row r="389"/>
+    <row r="390"/>
+    <row r="391"/>
+    <row r="392"/>
+    <row r="393"/>
+    <row r="394"/>
+    <row r="395"/>
+    <row r="396"/>
+    <row r="397"/>
+    <row r="398"/>
+    <row r="399"/>
+    <row r="400"/>
+    <row r="401"/>
+    <row r="402"/>
+    <row r="403"/>
+    <row r="404"/>
+    <row r="405"/>
+    <row r="406"/>
+    <row r="407"/>
+    <row r="408"/>
+    <row r="409"/>
+    <row r="410"/>
+    <row r="411"/>
+    <row r="412"/>
+    <row r="413"/>
+    <row r="414"/>
+    <row r="415"/>
+    <row r="416"/>
+    <row r="417"/>
+    <row r="418"/>
+    <row r="419"/>
+    <row r="420"/>
+    <row r="421"/>
+    <row r="422"/>
+    <row r="423"/>
+    <row r="424"/>
+    <row r="425"/>
+    <row r="426"/>
+    <row r="427"/>
+    <row r="428"/>
+    <row r="429"/>
+    <row r="430"/>
+    <row r="431"/>
+    <row r="432"/>
+    <row r="433"/>
+    <row r="434"/>
+    <row r="435"/>
+    <row r="436"/>
+    <row r="437"/>
+    <row r="438"/>
+    <row r="439"/>
+    <row r="440"/>
+    <row r="441"/>
+    <row r="442"/>
+    <row r="443"/>
+    <row r="444"/>
+    <row r="445"/>
+    <row r="446"/>
+    <row r="447"/>
+    <row r="448"/>
+    <row r="449"/>
+    <row r="450"/>
+    <row r="451"/>
+    <row r="452"/>
+    <row r="453"/>
+    <row r="454"/>
+    <row r="455"/>
+    <row r="456"/>
+    <row r="457"/>
+    <row r="458"/>
+    <row r="459"/>
+    <row r="460"/>
+    <row r="461"/>
+    <row r="462"/>
+    <row r="463"/>
+    <row r="464"/>
+    <row r="465"/>
+    <row r="466"/>
+    <row r="467"/>
+    <row r="468"/>
+    <row r="469"/>
+    <row r="470"/>
+    <row r="471"/>
+    <row r="472"/>
+    <row r="473"/>
+    <row r="474"/>
+    <row r="475"/>
+    <row r="476"/>
+    <row r="477"/>
+    <row r="478"/>
+    <row r="479"/>
+    <row r="480"/>
+    <row r="481"/>
+    <row r="482"/>
+    <row r="483"/>
+    <row r="484"/>
+    <row r="485"/>
+    <row r="486"/>
+    <row r="487"/>
+    <row r="488"/>
+    <row r="489"/>
+    <row r="490"/>
+    <row r="491"/>
+    <row r="492"/>
+    <row r="493"/>
+    <row r="494"/>
+    <row r="495"/>
+    <row r="496"/>
+    <row r="497"/>
+    <row r="498"/>
+    <row r="499"/>
+    <row r="500"/>
+    <row r="501"/>
+    <row r="502"/>
+    <row r="503"/>
+    <row r="504"/>
+    <row r="505"/>
+    <row r="506"/>
+    <row r="507"/>
+    <row r="508"/>
+    <row r="509"/>
+    <row r="510"/>
+    <row r="511"/>
+    <row r="512"/>
+    <row r="513"/>
+    <row r="514"/>
+    <row r="515"/>
+    <row r="516"/>
+    <row r="517"/>
+    <row r="518"/>
+    <row r="519"/>
+    <row r="520"/>
+    <row r="521"/>
+    <row r="522"/>
+    <row r="523"/>
+    <row r="524"/>
+    <row r="525"/>
+    <row r="526"/>
+    <row r="527"/>
+    <row r="528"/>
+    <row r="529"/>
+    <row r="530"/>
+    <row r="531"/>
+    <row r="532"/>
+    <row r="533"/>
+    <row r="534"/>
+    <row r="535"/>
+    <row r="536"/>
+    <row r="537"/>
+    <row r="538"/>
+    <row r="539"/>
+    <row r="540"/>
+    <row r="541"/>
+    <row r="542"/>
+    <row r="543"/>
+    <row r="544"/>
+    <row r="545"/>
+    <row r="546"/>
+    <row r="547"/>
+    <row r="548"/>
+    <row r="549"/>
+    <row r="550"/>
+    <row r="551"/>
+    <row r="552"/>
+    <row r="553"/>
+    <row r="554"/>
+    <row r="555"/>
+    <row r="556"/>
+    <row r="557"/>
+    <row r="558"/>
+    <row r="559"/>
+    <row r="560"/>
+    <row r="561"/>
+    <row r="562"/>
+    <row r="563"/>
+    <row r="564"/>
+    <row r="565"/>
+    <row r="566"/>
+    <row r="567"/>
+    <row r="568"/>
+    <row r="569"/>
+    <row r="570"/>
+    <row r="571"/>
+    <row r="572"/>
+    <row r="573"/>
+    <row r="574"/>
+    <row r="575"/>
+    <row r="576"/>
+    <row r="577"/>
+    <row r="578"/>
+    <row r="579"/>
+    <row r="580"/>
+    <row r="581"/>
+    <row r="582"/>
+    <row r="583"/>
+    <row r="584"/>
+    <row r="585"/>
+    <row r="586"/>
+    <row r="587"/>
+    <row r="588"/>
+    <row r="589"/>
+    <row r="590"/>
+    <row r="591"/>
+    <row r="592"/>
+    <row r="593"/>
+    <row r="594"/>
+    <row r="595"/>
+    <row r="596"/>
+    <row r="597"/>
+    <row r="598"/>
+    <row r="599"/>
+    <row r="600"/>
+    <row r="601"/>
+    <row r="602"/>
+    <row r="603"/>
+    <row r="604"/>
+    <row r="605"/>
+    <row r="606"/>
+    <row r="607"/>
+    <row r="608"/>
+    <row r="609"/>
+    <row r="610"/>
+    <row r="611"/>
+    <row r="612"/>
+    <row r="613"/>
+    <row r="614"/>
+    <row r="615"/>
+    <row r="616"/>
+    <row r="617"/>
+    <row r="618"/>
+    <row r="619"/>
+    <row r="620"/>
+    <row r="621"/>
+    <row r="622"/>
+    <row r="623"/>
+    <row r="624"/>
+    <row r="625"/>
+    <row r="626"/>
+    <row r="627"/>
+    <row r="628"/>
+    <row r="629"/>
+    <row r="630"/>
+    <row r="631"/>
+    <row r="632"/>
+    <row r="633"/>
+    <row r="634"/>
+    <row r="635"/>
+    <row r="636"/>
+    <row r="637"/>
+    <row r="638"/>
+    <row r="639"/>
+    <row r="640"/>
+    <row r="641"/>
+    <row r="642"/>
+    <row r="643"/>
+    <row r="644"/>
+    <row r="645"/>
+    <row r="646"/>
+    <row r="647"/>
+    <row r="648"/>
+    <row r="649"/>
+    <row r="650"/>
+    <row r="651"/>
+    <row r="652"/>
+    <row r="653"/>
+    <row r="654"/>
+    <row r="655"/>
+    <row r="656"/>
+    <row r="657"/>
+    <row r="658"/>
+    <row r="659"/>
+    <row r="660"/>
+    <row r="661"/>
+    <row r="662"/>
+    <row r="663"/>
+    <row r="664"/>
+    <row r="665"/>
+    <row r="666"/>
+    <row r="667"/>
+    <row r="668"/>
+    <row r="669"/>
+    <row r="670"/>
+    <row r="671"/>
+    <row r="672"/>
+    <row r="673"/>
+    <row r="674"/>
+    <row r="675"/>
+    <row r="676"/>
+    <row r="677"/>
+    <row r="678"/>
+    <row r="679"/>
+    <row r="680"/>
+    <row r="681"/>
+    <row r="682"/>
+    <row r="683"/>
+    <row r="684"/>
+    <row r="685"/>
+    <row r="686"/>
+    <row r="687"/>
+    <row r="688"/>
+    <row r="689"/>
+    <row r="690"/>
+    <row r="691"/>
+    <row r="692"/>
+    <row r="693"/>
+    <row r="694"/>
+    <row r="695"/>
+    <row r="696"/>
+    <row r="697"/>
+    <row r="698"/>
+    <row r="699"/>
+    <row r="700"/>
+    <row r="701"/>
+    <row r="702"/>
+    <row r="703"/>
+    <row r="704"/>
+    <row r="705"/>
+    <row r="706"/>
+    <row r="707"/>
+    <row r="708"/>
+    <row r="709"/>
+    <row r="710"/>
+    <row r="711"/>
+    <row r="712"/>
+    <row r="713"/>
+    <row r="714"/>
+    <row r="715"/>
+    <row r="716"/>
+    <row r="717"/>
+    <row r="718"/>
+    <row r="719"/>
+    <row r="720"/>
+    <row r="721"/>
+    <row r="722"/>
+    <row r="723"/>
+    <row r="724"/>
+    <row r="725"/>
+    <row r="726"/>
+    <row r="727"/>
+    <row r="728"/>
+    <row r="729"/>
+    <row r="730"/>
+    <row r="731"/>
+    <row r="732"/>
+    <row r="733"/>
+    <row r="734"/>
+    <row r="735"/>
+    <row r="736"/>
+    <row r="737"/>
+    <row r="738"/>
+    <row r="739"/>
+    <row r="740"/>
+    <row r="741"/>
+    <row r="742"/>
+    <row r="743"/>
+    <row r="744"/>
+    <row r="745"/>
+    <row r="746"/>
+    <row r="747"/>
+    <row r="748"/>
+    <row r="749"/>
+    <row r="750"/>
+    <row r="751"/>
+    <row r="752"/>
+    <row r="753"/>
+    <row r="754"/>
+    <row r="755"/>
+    <row r="756"/>
+    <row r="757"/>
+    <row r="758"/>
+    <row r="759"/>
+    <row r="760"/>
+    <row r="761"/>
+    <row r="762"/>
+    <row r="763"/>
+    <row r="764"/>
+    <row r="765"/>
+    <row r="766"/>
+    <row r="767"/>
+    <row r="768"/>
+    <row r="769"/>
+    <row r="770"/>
+    <row r="771"/>
+    <row r="772"/>
+    <row r="773"/>
+    <row r="774"/>
+    <row r="775"/>
+    <row r="776"/>
+    <row r="777"/>
+    <row r="778"/>
+    <row r="779"/>
+    <row r="780"/>
+    <row r="781"/>
+    <row r="782"/>
+    <row r="783"/>
+    <row r="784"/>
+    <row r="785"/>
+    <row r="786"/>
+    <row r="787"/>
+    <row r="788"/>
+    <row r="789"/>
+    <row r="790"/>
+    <row r="791"/>
+    <row r="792"/>
+    <row r="793"/>
+    <row r="794"/>
+    <row r="795"/>
+    <row r="796"/>
+    <row r="797"/>
+    <row r="798"/>
+    <row r="799"/>
+    <row r="800"/>
+    <row r="801"/>
+    <row r="802"/>
+    <row r="803"/>
+    <row r="804"/>
+    <row r="805"/>
+    <row r="806"/>
+    <row r="807"/>
+    <row r="808"/>
+    <row r="809"/>
+    <row r="810"/>
+    <row r="811"/>
+    <row r="812"/>
+    <row r="813"/>
+    <row r="814"/>
+    <row r="815"/>
+    <row r="816"/>
+    <row r="817"/>
+    <row r="818"/>
+    <row r="819"/>
+    <row r="820"/>
+    <row r="821"/>
+    <row r="822"/>
+    <row r="823"/>
+    <row r="824"/>
+    <row r="825"/>
+    <row r="826"/>
+    <row r="827"/>
+    <row r="828"/>
+    <row r="829"/>
+    <row r="830"/>
+    <row r="831"/>
+    <row r="832"/>
+    <row r="833"/>
+    <row r="834"/>
+    <row r="835"/>
+    <row r="836"/>
+    <row r="837"/>
+    <row r="838"/>
+    <row r="839"/>
+    <row r="840"/>
+    <row r="841"/>
+    <row r="842"/>
+    <row r="843"/>
+    <row r="844"/>
+    <row r="845"/>
+    <row r="846"/>
+    <row r="847"/>
+    <row r="848"/>
+    <row r="849"/>
+    <row r="850"/>
+    <row r="851"/>
+    <row r="852"/>
+    <row r="853"/>
+    <row r="854"/>
+    <row r="855"/>
+    <row r="856"/>
+    <row r="857"/>
+    <row r="858"/>
+    <row r="859"/>
+    <row r="860"/>
+    <row r="861"/>
+    <row r="862"/>
+    <row r="863"/>
+    <row r="864"/>
+    <row r="865"/>
+    <row r="866"/>
+    <row r="867"/>
+    <row r="868"/>
+    <row r="869"/>
+    <row r="870"/>
+    <row r="871"/>
+    <row r="872"/>
+    <row r="873"/>
+    <row r="874"/>
+    <row r="875"/>
+    <row r="876"/>
+    <row r="877"/>
+    <row r="878"/>
+    <row r="879"/>
+    <row r="880"/>
+    <row r="881"/>
+    <row r="882"/>
+    <row r="883"/>
+    <row r="884"/>
+    <row r="885"/>
+    <row r="886"/>
+    <row r="887"/>
+    <row r="888"/>
+    <row r="889"/>
+    <row r="890"/>
+    <row r="891"/>
+    <row r="892"/>
+    <row r="893"/>
+    <row r="894"/>
+    <row r="895"/>
+    <row r="896"/>
+    <row r="897"/>
+    <row r="898"/>
+    <row r="899"/>
+    <row r="900"/>
+    <row r="901"/>
+    <row r="902"/>
+    <row r="903"/>
+    <row r="904"/>
+    <row r="905"/>
+    <row r="906"/>
+    <row r="907"/>
+    <row r="908"/>
+    <row r="909"/>
+    <row r="910"/>
+    <row r="911"/>
+    <row r="912"/>
+    <row r="913"/>
+    <row r="914"/>
+    <row r="915"/>
+    <row r="916"/>
+    <row r="917"/>
+    <row r="918"/>
+    <row r="919"/>
+    <row r="920"/>
+    <row r="921"/>
+    <row r="922"/>
+    <row r="923"/>
+    <row r="924"/>
+    <row r="925"/>
+    <row r="926"/>
+    <row r="927"/>
+    <row r="928"/>
+    <row r="929"/>
+    <row r="930"/>
+    <row r="931"/>
+    <row r="932"/>
+    <row r="933"/>
+    <row r="934"/>
+    <row r="935"/>
+    <row r="936"/>
+    <row r="937"/>
+    <row r="938"/>
+    <row r="939"/>
+    <row r="940"/>
+    <row r="941"/>
+    <row r="942"/>
+    <row r="943"/>
+    <row r="944"/>
+    <row r="945"/>
+    <row r="946"/>
+    <row r="947"/>
+    <row r="948"/>
+    <row r="949"/>
+    <row r="950"/>
+    <row r="951"/>
+    <row r="952"/>
+    <row r="953"/>
+    <row r="954"/>
+    <row r="955"/>
+    <row r="956"/>
+    <row r="957"/>
+    <row r="958"/>
+    <row r="959"/>
+    <row r="960"/>
+    <row r="961"/>
+    <row r="962"/>
+    <row r="963"/>
+    <row r="964"/>
+    <row r="965"/>
+    <row r="966"/>
+    <row r="967"/>
+    <row r="968"/>
+    <row r="969"/>
+    <row r="970"/>
+    <row r="971"/>
+    <row r="972"/>
+    <row r="973"/>
+    <row r="974"/>
+    <row r="975"/>
+    <row r="976"/>
+    <row r="977"/>
+    <row r="978"/>
+    <row r="979"/>
+    <row r="980"/>
+    <row r="981"/>
+    <row r="982"/>
+    <row r="983"/>
+    <row r="984"/>
+    <row r="985"/>
+    <row r="986"/>
+    <row r="987"/>
+    <row r="988"/>
+    <row r="989"/>
+    <row r="990"/>
+    <row r="991"/>
+    <row r="992"/>
+    <row r="993"/>
+    <row r="994"/>
+    <row r="995"/>
+    <row r="996"/>
+    <row r="997"/>
+    <row r="998"/>
+    <row r="999"/>
+    <row r="1000"/>
+    <row r="1001"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="E2:E1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Status" error="Please select a valid status" type="list">
+    <dataValidation sqref="E2 E3 E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57 E58 E59 E60 E61 E62 E63 E64 E65 E66 E67 E68 E69 E70 E71 E72 E73 E74 E75 E76 E77 E78 E79 E80 E81 E82 E83 E84 E85 E86 E87 E88 E89 E90 E91 E92 E93 E94 E95 E96 E97 E98 E99 E100 E101 E102 E103 E104 E105 E106 E107 E108 E109 E110 E111 E112 E113 E114 E115 E116 E117 E118 E119 E120 E121 E122 E123 E124 E125 E126 E127 E128 E129 E130 E131 E132 E133 E134 E135 E136 E137 E138 E139 E140 E141 E142 E143 E144 E145 E146 E147 E148 E149 E150 E151 E152 E153 E154 E155 E156 E157 E158 E159 E160 E161 E162 E163 E164 E165 E166 E167 E168 E169 E170 E171 E172 E173 E174 E175 E176 E177 E178 E179 E180 E181 E182 E183 E184 E185 E186 E187 E188 E189 E190 E191 E192 E193 E194 E195 E196 E197 E198 E199 E200 E201 E202 E203 E204 E205 E206 E207 E208 E209 E210 E211 E212 E213 E214 E215 E216 E217 E218 E219 E220 E221 E222 E223 E224 E225 E226 E227 E228 E229 E230 E231 E232 E233 E234 E235 E236 E237 E238 E239 E240 E241 E242 E243 E244 E245 E246 E247 E248 E249 E250 E251 E252 E253 E254 E255 E256 E257 E258 E259 E260 E261 E262 E263 E264 E265 E266 E267 E268 E269 E270 E271 E272 E273 E274 E275 E276 E277 E278 E279 E280 E281 E282 E283 E284 E285 E286 E287 E288 E289 E290 E291 E292 E293 E294 E295 E296 E297 E298 E299 E300 E301 E302 E303 E304 E305 E306 E307 E308 E309 E310 E311 E312 E313 E314 E315 E316 E317 E318 E319 E320 E321 E322 E323 E324 E325 E326 E327 E328 E329 E330 E331 E332 E333 E334 E335 E336 E337 E338 E339 E340 E341 E342 E343 E344 E345 E346 E347 E348 E349 E350 E351 E352 E353 E354 E355 E356 E357 E358 E359 E360 E361 E362 E363 E364 E365 E366 E367 E368 E369 E370 E371 E372 E373 E374 E375 E376 E377 E378 E379 E380 E381 E382 E383 E384 E385 E386 E387 E388 E389 E390 E391 E392 E393 E394 E395 E396 E397 E398 E399 E400 E401 E402 E403 E404 E405 E406 E407 E408 E409 E410 E411 E412 E413 E414 E415 E416 E417 E418 E419 E420 E421 E422 E423 E424 E425 E426 E427 E428 E429 E430 E431 E432 E433 E434 E435 E436 E437 E438 E439 E440 E441 E442 E443 E444 E445 E446 E447 E448 E449 E450 E451 E452 E453 E454 E455 E456 E457 E458 E459 E460 E461 E462 E463 E464 E465 E466 E467 E468 E469 E470 E471 E472 E473 E474 E475 E476 E477 E478 E479 E480 E481 E482 E483 E484 E485 E486 E487 E488 E489 E490 E491 E492 E493 E494 E495 E496 E497 E498 E499 E500 E501 E502 E503 E504 E505 E506 E507 E508 E509 E510 E511 E512 E513 E514 E515 E516 E517 E518 E519 E520 E521 E522 E523 E524 E525 E526 E527 E528 E529 E530 E531 E532 E533 E534 E535 E536 E537 E538 E539 E540 E541 E542 E543 E544 E545 E546 E547 E548 E549 E550 E551 E552 E553 E554 E555 E556 E557 E558 E559 E560 E561 E562 E563 E564 E565 E566 E567 E568 E569 E570 E571 E572 E573 E574 E575 E576 E577 E578 E579 E580 E581 E582 E583 E584 E585 E586 E587 E588 E589 E590 E591 E592 E593 E594 E595 E596 E597 E598 E599 E600 E601 E602 E603 E604 E605 E606 E607 E608 E609 E610 E611 E612 E613 E614 E615 E616 E617 E618 E619 E620 E621 E622 E623 E624 E625 E626 E627 E628 E629 E630 E631 E632 E633 E634 E635 E636 E637 E638 E639 E640 E641 E642 E643 E644 E645 E646 E647 E648 E649 E650 E651 E652 E653 E654 E655 E656 E657 E658 E659 E660 E661 E662 E663 E664 E665 E666 E667 E668 E669 E670 E671 E672 E673 E674 E675 E676 E677 E678 E679 E680 E681 E682 E683 E684 E685 E686 E687 E688 E689 E690 E691 E692 E693 E694 E695 E696 E697 E698 E699 E700 E701 E702 E703 E704 E705 E706 E707 E708 E709 E710 E711 E712 E713 E714 E715 E716 E717 E718 E719 E720 E721 E722 E723 E724 E725 E726 E727 E728 E729 E730 E731 E732 E733 E734 E735 E736 E737 E738 E739 E740 E741 E742 E743 E744 E745 E746 E747 E748 E749 E750 E751 E752 E753 E754 E755 E756 E757 E758 E759 E760 E761 E762 E763 E764 E765 E766 E767 E768 E769 E770 E771 E772 E773 E774 E775 E776 E777 E778 E779 E780 E781 E782 E783 E784 E785 E786 E787 E788 E789 E790 E791 E792 E793 E794 E795 E796 E797 E798 E799 E800 E801 E802 E803 E804 E805 E806 E807 E808 E809 E810 E811 E812 E813 E814 E815 E816 E817 E818 E819 E820 E821 E822 E823 E824 E825 E826 E827 E828 E829 E830 E831 E832 E833 E834 E835 E836 E837 E838 E839 E840 E841 E842 E843 E844 E845 E846 E847 E848 E849 E850 E851 E852 E853 E854 E855 E856 E857 E858 E859 E860 E861 E862 E863 E864 E865 E866 E867 E868 E869 E870 E871 E872 E873 E874 E875 E876 E877 E878 E879 E880 E881 E882 E883 E884 E885 E886 E887 E888 E889 E890 E891 E892 E893 E894 E895 E896 E897 E898 E899 E900 E901 E902 E903 E904 E905 E906 E907 E908 E909 E910 E911 E912 E913 E914 E915 E916 E917 E918 E919 E920 E921 E922 E923 E924 E925 E926 E927 E928 E929 E930 E931 E932 E933 E934 E935 E936 E937 E938 E939 E940 E941 E942 E943 E944 E945 E946 E947 E948 E949 E950 E951 E952 E953 E954 E955 E956 E957 E958 E959 E960 E961 E962 E963 E964 E965 E966 E967 E968 E969 E970 E971 E972 E973 E974 E975 E976 E977 E978 E979 E980 E981 E982 E983 E984 E985 E986 E987 E988 E989 E990 E991 E992 E993 E994 E995 E996 E997 E998 E999 E1000 E1001" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" error="Please select a valid status" type="list">
       <formula1>"uploaded,transcribing,mapping,review,approved,sent,error"</formula1>
     </dataValidation>
   </dataValidations>
@@ -745,10 +1707,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -770,7 +1732,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>class_period</t>
+          <t>section</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -800,9 +1762,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
@@ -866,10 +1828,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -919,16 +1881,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-    <col width="40" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="40" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="28" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
     <col width="14" customWidth="1" min="11" max="11"/>
     <col width="14" customWidth="1" min="12" max="12"/>
   </cols>
@@ -1031,126 +1993,84 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="120" customHeight="1">
+    <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>SPEAKER_IDENTIFICATION</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>You are analyzing the beginning of a classroom Harkness discussion recording.
-Students typically introduce themselves at the start. Listen for patterns like:
-- "Hi, I'm [name]"
-- "My name is [name]"
-- "This is [name]"
-- "[Name] here"
-- Other natural introductions
-Analyze this transcript excerpt and identify which speaker label corresponds to which student name.
-IMPORTANT RULES:
-1. Only include speakers you can confidently identify from explicit introductions
-2. If a speaker cannot be identified, map them to "?" instead
-3. Be case-sensitive with names as they appear
-4. The teacher may also speak — if identified, include them as "Teacher"
-Return ONLY a valid JSON object mapping speaker labels to names.
-Example format: {"Speaker 0": "Maria", "Speaker 1": "James", "Speaker 2": "Teacher", "Speaker 3": "?"}
-Transcript excerpt:
-{transcript}
-JSON mapping:</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="120" customHeight="1">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DISCUSSION_SUMMARY</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Summarize this Harkness discussion for the teacher's records.
-Include:
-1. **Main themes/topics** discussed (2-3 bullet points)
-2. **Key insights** that emerged from the discussion
-3. **Discussion quality** assessment (engagement level, depth of analysis)
-4. **Notable moments** (breakthrough insights, good collaboration, etc.)
-Keep the summary to about 150-200 words.
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Analyze the following transcript excerpt from a classroom discussion. Students typically introduce themselves at the beginning. Identify each speaker by matching their speaker label to their name.
 Transcript:
 {transcript}
-Discussion Summary:</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="120" customHeight="1">
+Return a JSON object mapping speaker labels to student names. Use "?" for unidentified speakers and "Teacher" for the teacher. Example: {"Speaker 0": "Maria", "Speaker 1": "Teacher", "Speaker 2": "?"}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DISCUSSION_SUMMARY</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Summarize the following Harkness discussion in 2-3 paragraphs. Focus on the main topics discussed, key arguments made, and the overall quality of student engagement.
+Transcript:
+{transcript}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>GROUP_FEEDBACK</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Generate feedback for the whole class based on their Harkness discussion.
-The teacher gave this discussion a grade of {grade}.
-Teacher's notes/feedback:
-{teacher_feedback}
-Discussion transcript:
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>You are a high school teacher providing feedback on a Harkness discussion. Write a constructive feedback paragraph for the class based on their discussion.
+Transcript:
 {transcript}
-Write a supportive but honest group feedback paragraph (4-6 sentences) that:
-1. Summarizes the overall quality of the discussion
-2. Highlights specific strong moments or contributions
-3. Identifies areas where the class can improve their discussion skills
-4. Connects to Harkness discussion values (collaboration, evidence-based reasoning, building on others' ideas)
-5. Ends on an encouraging note
-Group feedback:</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="120" customHeight="1">
+Grade: {grade}
+Teacher notes: {teacher_feedback}
+Provide specific, encouraging feedback that references actual moments from the discussion. Keep it to 1-2 paragraphs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>INDIVIDUAL_FEEDBACK</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Generate personalized feedback for {student_name} based on their Harkness discussion participation.
-The teacher gave this student a grade of {grade}.
-Teacher's notes/feedback:
-{teacher_feedback}
-{student_name}'s contributions from the transcript:
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>You are a high school teacher providing personalized feedback to a student about their Harkness discussion participation.
+Student: {student_name}
+Their contributions:
 {contributions}
 Full discussion transcript (for context):
 {transcript}
-Write a supportive but honest feedback paragraph (3-5 sentences) that:
-1. Acknowledges specific strengths from their participation
-2. References actual points they made when notable
-3. Provides one concrete suggestion for growth
-4. Ends on an encouraging note
-Feedback for {student_name}:</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="120" customHeight="1">
+Grade: {grade}
+Teacher notes: {teacher_feedback}
+Write a brief, constructive, personalized feedback paragraph for this student. Reference specific things they said. Keep it to 1-2 paragraphs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>TEACHER_FEEDBACK_EXTRACTION</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>You are analyzing a Harkness discussion transcript.
-At the end of many discussions, the teacher provides verbal feedback to the class. This typically includes:
-- Overall assessment of the discussion quality
-- Highlights of good contributions
-- Areas for improvement
-- Specific student callouts (positive or constructive)
-Extract ONLY the teacher's feedback section from this transcript.
-This is usually near the end, after the main discussion concludes.
-If there is no clear teacher feedback section, return "NO_FEEDBACK_FOUND".
-Return ONLY the teacher feedback text, nothing else.
-Full transcript:
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Analyze this discussion transcript and extract any verbal feedback the teacher gave during or after the discussion. Look for the teacher summarizing the discussion, giving praise, or offering critique.
+Transcript:
 {transcript}
-Teacher feedback:</t>
+If the teacher gave verbal feedback, return it as a summary. If no teacher feedback is found, return exactly: NO_FEEDBACK_FOUND</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Canvas assignment vs discussion topic support
- Add `canvas_item_type` setting (assignment/discussion) and per-discussion
  override column so teachers can use Canvas discussion topic IDs
- Add `resolveCanvasAssignmentId()` to auto-resolve discussion topic IDs
  to their linked assignment IDs via the Canvas API before grade posting
- Update `fetchCanvasCourseData()` to fetch and display both assignments
  and graded discussion topics in the course data dialog
- Add dropdown validation for canvas_item_type on the Discussions sheet
- Regenerate template.xlsx with new column and setting

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -574,6 +574,18 @@
       </c>
       <c r="B12" t="inlineStr"/>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>canvas_item_type</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>assignment</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -585,7 +597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1001"/>
+  <dimension ref="A1:O1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -605,9 +617,10 @@
     <col width="22" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
     <col width="24" customWidth="1" min="11" max="11"/>
-    <col width="17" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="17" customWidth="1" min="13" max="13"/>
     <col width="14" customWidth="1" min="14" max="14"/>
+    <col width="14" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -668,15 +681,20 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>canvas_item_type</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>error_message</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>created_at</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
         </is>
@@ -1683,9 +1701,12 @@
     <row r="1000"/>
     <row r="1001"/>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="E2 E3 E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57 E58 E59 E60 E61 E62 E63 E64 E65 E66 E67 E68 E69 E70 E71 E72 E73 E74 E75 E76 E77 E78 E79 E80 E81 E82 E83 E84 E85 E86 E87 E88 E89 E90 E91 E92 E93 E94 E95 E96 E97 E98 E99 E100 E101 E102 E103 E104 E105 E106 E107 E108 E109 E110 E111 E112 E113 E114 E115 E116 E117 E118 E119 E120 E121 E122 E123 E124 E125 E126 E127 E128 E129 E130 E131 E132 E133 E134 E135 E136 E137 E138 E139 E140 E141 E142 E143 E144 E145 E146 E147 E148 E149 E150 E151 E152 E153 E154 E155 E156 E157 E158 E159 E160 E161 E162 E163 E164 E165 E166 E167 E168 E169 E170 E171 E172 E173 E174 E175 E176 E177 E178 E179 E180 E181 E182 E183 E184 E185 E186 E187 E188 E189 E190 E191 E192 E193 E194 E195 E196 E197 E198 E199 E200 E201 E202 E203 E204 E205 E206 E207 E208 E209 E210 E211 E212 E213 E214 E215 E216 E217 E218 E219 E220 E221 E222 E223 E224 E225 E226 E227 E228 E229 E230 E231 E232 E233 E234 E235 E236 E237 E238 E239 E240 E241 E242 E243 E244 E245 E246 E247 E248 E249 E250 E251 E252 E253 E254 E255 E256 E257 E258 E259 E260 E261 E262 E263 E264 E265 E266 E267 E268 E269 E270 E271 E272 E273 E274 E275 E276 E277 E278 E279 E280 E281 E282 E283 E284 E285 E286 E287 E288 E289 E290 E291 E292 E293 E294 E295 E296 E297 E298 E299 E300 E301 E302 E303 E304 E305 E306 E307 E308 E309 E310 E311 E312 E313 E314 E315 E316 E317 E318 E319 E320 E321 E322 E323 E324 E325 E326 E327 E328 E329 E330 E331 E332 E333 E334 E335 E336 E337 E338 E339 E340 E341 E342 E343 E344 E345 E346 E347 E348 E349 E350 E351 E352 E353 E354 E355 E356 E357 E358 E359 E360 E361 E362 E363 E364 E365 E366 E367 E368 E369 E370 E371 E372 E373 E374 E375 E376 E377 E378 E379 E380 E381 E382 E383 E384 E385 E386 E387 E388 E389 E390 E391 E392 E393 E394 E395 E396 E397 E398 E399 E400 E401 E402 E403 E404 E405 E406 E407 E408 E409 E410 E411 E412 E413 E414 E415 E416 E417 E418 E419 E420 E421 E422 E423 E424 E425 E426 E427 E428 E429 E430 E431 E432 E433 E434 E435 E436 E437 E438 E439 E440 E441 E442 E443 E444 E445 E446 E447 E448 E449 E450 E451 E452 E453 E454 E455 E456 E457 E458 E459 E460 E461 E462 E463 E464 E465 E466 E467 E468 E469 E470 E471 E472 E473 E474 E475 E476 E477 E478 E479 E480 E481 E482 E483 E484 E485 E486 E487 E488 E489 E490 E491 E492 E493 E494 E495 E496 E497 E498 E499 E500 E501 E502 E503 E504 E505 E506 E507 E508 E509 E510 E511 E512 E513 E514 E515 E516 E517 E518 E519 E520 E521 E522 E523 E524 E525 E526 E527 E528 E529 E530 E531 E532 E533 E534 E535 E536 E537 E538 E539 E540 E541 E542 E543 E544 E545 E546 E547 E548 E549 E550 E551 E552 E553 E554 E555 E556 E557 E558 E559 E560 E561 E562 E563 E564 E565 E566 E567 E568 E569 E570 E571 E572 E573 E574 E575 E576 E577 E578 E579 E580 E581 E582 E583 E584 E585 E586 E587 E588 E589 E590 E591 E592 E593 E594 E595 E596 E597 E598 E599 E600 E601 E602 E603 E604 E605 E606 E607 E608 E609 E610 E611 E612 E613 E614 E615 E616 E617 E618 E619 E620 E621 E622 E623 E624 E625 E626 E627 E628 E629 E630 E631 E632 E633 E634 E635 E636 E637 E638 E639 E640 E641 E642 E643 E644 E645 E646 E647 E648 E649 E650 E651 E652 E653 E654 E655 E656 E657 E658 E659 E660 E661 E662 E663 E664 E665 E666 E667 E668 E669 E670 E671 E672 E673 E674 E675 E676 E677 E678 E679 E680 E681 E682 E683 E684 E685 E686 E687 E688 E689 E690 E691 E692 E693 E694 E695 E696 E697 E698 E699 E700 E701 E702 E703 E704 E705 E706 E707 E708 E709 E710 E711 E712 E713 E714 E715 E716 E717 E718 E719 E720 E721 E722 E723 E724 E725 E726 E727 E728 E729 E730 E731 E732 E733 E734 E735 E736 E737 E738 E739 E740 E741 E742 E743 E744 E745 E746 E747 E748 E749 E750 E751 E752 E753 E754 E755 E756 E757 E758 E759 E760 E761 E762 E763 E764 E765 E766 E767 E768 E769 E770 E771 E772 E773 E774 E775 E776 E777 E778 E779 E780 E781 E782 E783 E784 E785 E786 E787 E788 E789 E790 E791 E792 E793 E794 E795 E796 E797 E798 E799 E800 E801 E802 E803 E804 E805 E806 E807 E808 E809 E810 E811 E812 E813 E814 E815 E816 E817 E818 E819 E820 E821 E822 E823 E824 E825 E826 E827 E828 E829 E830 E831 E832 E833 E834 E835 E836 E837 E838 E839 E840 E841 E842 E843 E844 E845 E846 E847 E848 E849 E850 E851 E852 E853 E854 E855 E856 E857 E858 E859 E860 E861 E862 E863 E864 E865 E866 E867 E868 E869 E870 E871 E872 E873 E874 E875 E876 E877 E878 E879 E880 E881 E882 E883 E884 E885 E886 E887 E888 E889 E890 E891 E892 E893 E894 E895 E896 E897 E898 E899 E900 E901 E902 E903 E904 E905 E906 E907 E908 E909 E910 E911 E912 E913 E914 E915 E916 E917 E918 E919 E920 E921 E922 E923 E924 E925 E926 E927 E928 E929 E930 E931 E932 E933 E934 E935 E936 E937 E938 E939 E940 E941 E942 E943 E944 E945 E946 E947 E948 E949 E950 E951 E952 E953 E954 E955 E956 E957 E958 E959 E960 E961 E962 E963 E964 E965 E966 E967 E968 E969 E970 E971 E972 E973 E974 E975 E976 E977 E978 E979 E980 E981 E982 E983 E984 E985 E986 E987 E988 E989 E990 E991 E992 E993 E994 E995 E996 E997 E998 E999 E1000 E1001" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" error="Please select a valid status" type="list">
+  <dataValidations count="2">
+    <dataValidation sqref="E2 E3 E4 E5 E6 E7 E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25 E26 E27 E28 E29 E30 E31 E32 E33 E34 E35 E36 E37 E38 E39 E40 E41 E42 E43 E44 E45 E46 E47 E48 E49 E50 E51 E52 E53 E54 E55 E56 E57 E58 E59 E60 E61 E62 E63 E64 E65 E66 E67 E68 E69 E70 E71 E72 E73 E74 E75 E76 E77 E78 E79 E80 E81 E82 E83 E84 E85 E86 E87 E88 E89 E90 E91 E92 E93 E94 E95 E96 E97 E98 E99 E100 E101 E102 E103 E104 E105 E106 E107 E108 E109 E110 E111 E112 E113 E114 E115 E116 E117 E118 E119 E120 E121 E122 E123 E124 E125 E126 E127 E128 E129 E130 E131 E132 E133 E134 E135 E136 E137 E138 E139 E140 E141 E142 E143 E144 E145 E146 E147 E148 E149 E150 E151 E152 E153 E154 E155 E156 E157 E158 E159 E160 E161 E162 E163 E164 E165 E166 E167 E168 E169 E170 E171 E172 E173 E174 E175 E176 E177 E178 E179 E180 E181 E182 E183 E184 E185 E186 E187 E188 E189 E190 E191 E192 E193 E194 E195 E196 E197 E198 E199 E200 E201 E202 E203 E204 E205 E206 E207 E208 E209 E210 E211 E212 E213 E214 E215 E216 E217 E218 E219 E220 E221 E222 E223 E224 E225 E226 E227 E228 E229 E230 E231 E232 E233 E234 E235 E236 E237 E238 E239 E240 E241 E242 E243 E244 E245 E246 E247 E248 E249 E250 E251 E252 E253 E254 E255 E256 E257 E258 E259 E260 E261 E262 E263 E264 E265 E266 E267 E268 E269 E270 E271 E272 E273 E274 E275 E276 E277 E278 E279 E280 E281 E282 E283 E284 E285 E286 E287 E288 E289 E290 E291 E292 E293 E294 E295 E296 E297 E298 E299 E300 E301 E302 E303 E304 E305 E306 E307 E308 E309 E310 E311 E312 E313 E314 E315 E316 E317 E318 E319 E320 E321 E322 E323 E324 E325 E326 E327 E328 E329 E330 E331 E332 E333 E334 E335 E336 E337 E338 E339 E340 E341 E342 E343 E344 E345 E346 E347 E348 E349 E350 E351 E352 E353 E354 E355 E356 E357 E358 E359 E360 E361 E362 E363 E364 E365 E366 E367 E368 E369 E370 E371 E372 E373 E374 E375 E376 E377 E378 E379 E380 E381 E382 E383 E384 E385 E386 E387 E388 E389 E390 E391 E392 E393 E394 E395 E396 E397 E398 E399 E400 E401 E402 E403 E404 E405 E406 E407 E408 E409 E410 E411 E412 E413 E414 E415 E416 E417 E418 E419 E420 E421 E422 E423 E424 E425 E426 E427 E428 E429 E430 E431 E432 E433 E434 E435 E436 E437 E438 E439 E440 E441 E442 E443 E444 E445 E446 E447 E448 E449 E450 E451 E452 E453 E454 E455 E456 E457 E458 E459 E460 E461 E462 E463 E464 E465 E466 E467 E468 E469 E470 E471 E472 E473 E474 E475 E476 E477 E478 E479 E480 E481 E482 E483 E484 E485 E486 E487 E488 E489 E490 E491 E492 E493 E494 E495 E496 E497 E498 E499 E500 E501 E502 E503 E504 E505 E506 E507 E508 E509 E510 E511 E512 E513 E514 E515 E516 E517 E518 E519 E520 E521 E522 E523 E524 E525 E526 E527 E528 E529 E530 E531 E532 E533 E534 E535 E536 E537 E538 E539 E540 E541 E542 E543 E544 E545 E546 E547 E548 E549 E550 E551 E552 E553 E554 E555 E556 E557 E558 E559 E560 E561 E562 E563 E564 E565 E566 E567 E568 E569 E570 E571 E572 E573 E574 E575 E576 E577 E578 E579 E580 E581 E582 E583 E584 E585 E586 E587 E588 E589 E590 E591 E592 E593 E594 E595 E596 E597 E598 E599 E600 E601 E602 E603 E604 E605 E606 E607 E608 E609 E610 E611 E612 E613 E614 E615 E616 E617 E618 E619 E620 E621 E622 E623 E624 E625 E626 E627 E628 E629 E630 E631 E632 E633 E634 E635 E636 E637 E638 E639 E640 E641 E642 E643 E644 E645 E646 E647 E648 E649 E650 E651 E652 E653 E654 E655 E656 E657 E658 E659 E660 E661 E662 E663 E664 E665 E666 E667 E668 E669 E670 E671 E672 E673 E674 E675 E676 E677 E678 E679 E680 E681 E682 E683 E684 E685 E686 E687 E688 E689 E690 E691 E692 E693 E694 E695 E696 E697 E698 E699 E700 E701 E702 E703 E704 E705 E706 E707 E708 E709 E710 E711 E712 E713 E714 E715 E716 E717 E718 E719 E720 E721 E722 E723 E724 E725 E726 E727 E728 E729 E730 E731 E732 E733 E734 E735 E736 E737 E738 E739 E740 E741 E742 E743 E744 E745 E746 E747 E748 E749 E750 E751 E752 E753 E754 E755 E756 E757 E758 E759 E760 E761 E762 E763 E764 E765 E766 E767 E768 E769 E770 E771 E772 E773 E774 E775 E776 E777 E778 E779 E780 E781 E782 E783 E784 E785 E786 E787 E788 E789 E790 E791 E792 E793 E794 E795 E796 E797 E798 E799 E800 E801 E802 E803 E804 E805 E806 E807 E808 E809 E810 E811 E812 E813 E814 E815 E816 E817 E818 E819 E820 E821 E822 E823 E824 E825 E826 E827 E828 E829 E830 E831 E832 E833 E834 E835 E836 E837 E838 E839 E840 E841 E842 E843 E844 E845 E846 E847 E848 E849 E850 E851 E852 E853 E854 E855 E856 E857 E858 E859 E860 E861 E862 E863 E864 E865 E866 E867 E868 E869 E870 E871 E872 E873 E874 E875 E876 E877 E878 E879 E880 E881 E882 E883 E884 E885 E886 E887 E888 E889 E890 E891 E892 E893 E894 E895 E896 E897 E898 E899 E900 E901 E902 E903 E904 E905 E906 E907 E908 E909 E910 E911 E912 E913 E914 E915 E916 E917 E918 E919 E920 E921 E922 E923 E924 E925 E926 E927 E928 E929 E930 E931 E932 E933 E934 E935 E936 E937 E938 E939 E940 E941 E942 E943 E944 E945 E946 E947 E948 E949 E950 E951 E952 E953 E954 E955 E956 E957 E958 E959 E960 E961 E962 E963 E964 E965 E966 E967 E968 E969 E970 E971 E972 E973 E974 E975 E976 E977 E978 E979 E980 E981 E982 E983 E984 E985 E986 E987 E988 E989 E990 E991 E992 E993 E994 E995 E996 E997 E998 E999 E1000 E1001" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"uploaded,transcribing,mapping,review,approved,sent,error"</formula1>
+    </dataValidation>
+    <dataValidation sqref="L2 L3 L4 L5 L6 L7 L8 L9 L10 L11 L12 L13 L14 L15 L16 L17 L18 L19 L20 L21 L22 L23 L24 L25 L26 L27 L28 L29 L30 L31 L32 L33 L34 L35 L36 L37 L38 L39 L40 L41 L42 L43 L44 L45 L46 L47 L48 L49 L50 L51 L52 L53 L54 L55 L56 L57 L58 L59 L60 L61 L62 L63 L64 L65 L66 L67 L68 L69 L70 L71 L72 L73 L74 L75 L76 L77 L78 L79 L80 L81 L82 L83 L84 L85 L86 L87 L88 L89 L90 L91 L92 L93 L94 L95 L96 L97 L98 L99 L100 L101 L102 L103 L104 L105 L106 L107 L108 L109 L110 L111 L112 L113 L114 L115 L116 L117 L118 L119 L120 L121 L122 L123 L124 L125 L126 L127 L128 L129 L130 L131 L132 L133 L134 L135 L136 L137 L138 L139 L140 L141 L142 L143 L144 L145 L146 L147 L148 L149 L150 L151 L152 L153 L154 L155 L156 L157 L158 L159 L160 L161 L162 L163 L164 L165 L166 L167 L168 L169 L170 L171 L172 L173 L174 L175 L176 L177 L178 L179 L180 L181 L182 L183 L184 L185 L186 L187 L188 L189 L190 L191 L192 L193 L194 L195 L196 L197 L198 L199 L200 L201 L202 L203 L204 L205 L206 L207 L208 L209 L210 L211 L212 L213 L214 L215 L216 L217 L218 L219 L220 L221 L222 L223 L224 L225 L226 L227 L228 L229 L230 L231 L232 L233 L234 L235 L236 L237 L238 L239 L240 L241 L242 L243 L244 L245 L246 L247 L248 L249 L250 L251 L252 L253 L254 L255 L256 L257 L258 L259 L260 L261 L262 L263 L264 L265 L266 L267 L268 L269 L270 L271 L272 L273 L274 L275 L276 L277 L278 L279 L280 L281 L282 L283 L284 L285 L286 L287 L288 L289 L290 L291 L292 L293 L294 L295 L296 L297 L298 L299 L300 L301 L302 L303 L304 L305 L306 L307 L308 L309 L310 L311 L312 L313 L314 L315 L316 L317 L318 L319 L320 L321 L322 L323 L324 L325 L326 L327 L328 L329 L330 L331 L332 L333 L334 L335 L336 L337 L338 L339 L340 L341 L342 L343 L344 L345 L346 L347 L348 L349 L350 L351 L352 L353 L354 L355 L356 L357 L358 L359 L360 L361 L362 L363 L364 L365 L366 L367 L368 L369 L370 L371 L372 L373 L374 L375 L376 L377 L378 L379 L380 L381 L382 L383 L384 L385 L386 L387 L388 L389 L390 L391 L392 L393 L394 L395 L396 L397 L398 L399 L400 L401 L402 L403 L404 L405 L406 L407 L408 L409 L410 L411 L412 L413 L414 L415 L416 L417 L418 L419 L420 L421 L422 L423 L424 L425 L426 L427 L428 L429 L430 L431 L432 L433 L434 L435 L436 L437 L438 L439 L440 L441 L442 L443 L444 L445 L446 L447 L448 L449 L450 L451 L452 L453 L454 L455 L456 L457 L458 L459 L460 L461 L462 L463 L464 L465 L466 L467 L468 L469 L470 L471 L472 L473 L474 L475 L476 L477 L478 L479 L480 L481 L482 L483 L484 L485 L486 L487 L488 L489 L490 L491 L492 L493 L494 L495 L496 L497 L498 L499 L500 L501 L502 L503 L504 L505 L506 L507 L508 L509 L510 L511 L512 L513 L514 L515 L516 L517 L518 L519 L520 L521 L522 L523 L524 L525 L526 L527 L528 L529 L530 L531 L532 L533 L534 L535 L536 L537 L538 L539 L540 L541 L542 L543 L544 L545 L546 L547 L548 L549 L550 L551 L552 L553 L554 L555 L556 L557 L558 L559 L560 L561 L562 L563 L564 L565 L566 L567 L568 L569 L570 L571 L572 L573 L574 L575 L576 L577 L578 L579 L580 L581 L582 L583 L584 L585 L586 L587 L588 L589 L590 L591 L592 L593 L594 L595 L596 L597 L598 L599 L600 L601 L602 L603 L604 L605 L606 L607 L608 L609 L610 L611 L612 L613 L614 L615 L616 L617 L618 L619 L620 L621 L622 L623 L624 L625 L626 L627 L628 L629 L630 L631 L632 L633 L634 L635 L636 L637 L638 L639 L640 L641 L642 L643 L644 L645 L646 L647 L648 L649 L650 L651 L652 L653 L654 L655 L656 L657 L658 L659 L660 L661 L662 L663 L664 L665 L666 L667 L668 L669 L670 L671 L672 L673 L674 L675 L676 L677 L678 L679 L680 L681 L682 L683 L684 L685 L686 L687 L688 L689 L690 L691 L692 L693 L694 L695 L696 L697 L698 L699 L700 L701 L702 L703 L704 L705 L706 L707 L708 L709 L710 L711 L712 L713 L714 L715 L716 L717 L718 L719 L720 L721 L722 L723 L724 L725 L726 L727 L728 L729 L730 L731 L732 L733 L734 L735 L736 L737 L738 L739 L740 L741 L742 L743 L744 L745 L746 L747 L748 L749 L750 L751 L752 L753 L754 L755 L756 L757 L758 L759 L760 L761 L762 L763 L764 L765 L766 L767 L768 L769 L770 L771 L772 L773 L774 L775 L776 L777 L778 L779 L780 L781 L782 L783 L784 L785 L786 L787 L788 L789 L790 L791 L792 L793 L794 L795 L796 L797 L798 L799 L800 L801 L802 L803 L804 L805 L806 L807 L808 L809 L810 L811 L812 L813 L814 L815 L816 L817 L818 L819 L820 L821 L822 L823 L824 L825 L826 L827 L828 L829 L830 L831 L832 L833 L834 L835 L836 L837 L838 L839 L840 L841 L842 L843 L844 L845 L846 L847 L848 L849 L850 L851 L852 L853 L854 L855 L856 L857 L858 L859 L860 L861 L862 L863 L864 L865 L866 L867 L868 L869 L870 L871 L872 L873 L874 L875 L876 L877 L878 L879 L880 L881 L882 L883 L884 L885 L886 L887 L888 L889 L890 L891 L892 L893 L894 L895 L896 L897 L898 L899 L900 L901 L902 L903 L904 L905 L906 L907 L908 L909 L910 L911 L912 L913 L914 L915 L916 L917 L918 L919 L920 L921 L922 L923 L924 L925 L926 L927 L928 L929 L930 L931 L932 L933 L934 L935 L936 L937 L938 L939 L940 L941 L942 L943 L944 L945 L946 L947 L948 L949 L950 L951 L952 L953 L954 L955 L956 L957 L958 L959 L960 L961 L962 L963 L964 L965 L966 L967 L968 L969 L970 L971 L972 L973 L974 L975 L976 L977 L978 L979 L980 L981 L982 L983 L984 L985 L986 L987 L988 L989 L990 L991 L992 L993 L994 L995 L996 L997 L998 L999 L1000 L1001" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"assignment,discussion"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Consolidate prompts: remove DISCUSSION_SUMMARY and TEACHER_FEEDBACK_EXTRACTION
Both were redundant — GROUP_FEEDBACK P1 already produces the summary, and
both feedback prompts already receive the full transcript with instructions
to find teacher oral feedback. This removes 2 Gemini API calls per
discussion, the discussion_summary column from Discussions, and the
teacher_feedback column from Transcripts.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -615,7 +615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -632,13 +632,12 @@
     <col width="13" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
     <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="22" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="24" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
-    <col width="17" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="17" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
     <col width="14" customWidth="1" min="14" max="14"/>
-    <col width="14" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -684,35 +683,30 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>discussion_summary</t>
+          <t>approved</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>approved</t>
+          <t>canvas_assignment_id</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>canvas_assignment_id</t>
+          <t>canvas_item_type</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>canvas_item_type</t>
+          <t>error_message</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>error_message</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>created_at</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
         </is>
@@ -783,7 +777,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -796,9 +790,8 @@
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -824,15 +817,10 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>teacher_feedback</t>
+          <t>created_at</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>created_at</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>updated_at</t>
         </is>
@@ -999,7 +987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1008,7 +996,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="31" customWidth="1" min="1" max="1"/>
+    <col width="26" customWidth="1" min="1" max="1"/>
     <col width="100" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -1056,31 +1044,10 @@
     <row r="3" ht="200" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>DISCUSSION_SUMMARY</t>
+          <t>GROUP_FEEDBACK</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Summarize this Harkness discussion for the teacher's records.
-Include:
-1. **Main themes/topics** discussed (2-3 bullet points)
-2. **Key insights** that emerged from the discussion
-3. **Discussion quality** assessment (engagement level, depth of analysis)
-4. **Notable moments** (breakthrough insights, good collaboration, etc.)
-Keep the summary to about 150-200 words.
-Transcript:
-{transcript}
-Discussion Summary:</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="200" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>GROUP_FEEDBACK</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>You are a high school teacher analyzing a Harkness discussion. You will produce exactly two paragraphs.
 **PARAGRAPH 1 — Discussion Summary** (Neutral Voice)
@@ -1100,20 +1067,19 @@
 - Credit specific students by name for notable contributions.
 - If the teacher intervened to guide the discussion, acknowledge this (e.g., "I had to provide the key synthesizing question").
 Grade: {grade}
-Teacher's notes: {teacher_feedback}
 Transcript:
 {transcript}
 Write the two paragraphs now (summary paragraph first, then evaluative comment):</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="200" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
+    <row r="4" ht="200" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>INDIVIDUAL_FEEDBACK</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>You are a high school teacher providing personalized feedback to {student_name} about their Harkness discussion participation. You will produce exactly two paragraphs.
 **PARAGRAPH 1 — Contribution Summary** (Neutral Voice)
@@ -1128,8 +1094,9 @@
 - High grade (9-10): "Excellent" contributions; the gap is a stretch goal.
 - Medium grade (7-8.5): "Solid" participation with clear room to grow.
 - Lower grade (below 7): Encouraging but honest about what's missing.
+**Important:**
+- If the teacher gave oral feedback during the discussion (often near the end — look for phrases like "my evaluation," "my feedback," or the teacher summarizing), align your evaluation with their points.
 Grade: {grade}
-Teacher's notes: {teacher_feedback}
 {student_name}'s contributions:
 {contributions}
 Full discussion transcript (for context):
@@ -1138,28 +1105,6 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="200" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>TEACHER_FEEDBACK_EXTRACTION</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>You are analyzing a Harkness discussion transcript.
-The teacher typically gives an oral evaluative comment near the end of the discussion. Look for:
-- Phrases like "my evaluation of the discussion," "my feedback," "my evaluative comment," "let me say a few things about today"
-- The teacher summarizing, giving praise, or offering critique after the main discussion concludes
-- This may be split across multiple teacher comments or not explicitly labeled
-Extract and summarize the teacher's oral evaluative feedback.
-If there is no clear teacher feedback, return "NO_FEEDBACK_FOUND".
-Return ONLY the teacher's feedback, nothing else.
-Full transcript:
-{transcript}
-Teacher feedback:</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>